<commit_message>
- API (done) - UI (wip)
</commit_message>
<xml_diff>
--- a/PORECT.API/Template/Template Report.xlsx
+++ b/PORECT.API/Template/Template Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThinkPad\source\repos\InterviewSwapro\PORECT.API\Template\Lumpsum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThinkPad\source\repos\InterviewSwapro\PORECT.API\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C35543-29D6-4DE0-A426-49E4B9D649E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5BE9D0-A347-468E-AEA9-C32B94607477}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>Periode : [Indonesian month] [year]</t>
-  </si>
-  <si>
     <t>ROOM NAME</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>TOTAL DURATION</t>
+  </si>
+  <si>
+    <t>Periode : [Month description] [year]</t>
   </si>
 </sst>
 </file>
@@ -462,7 +462,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -494,7 +494,7 @@
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -519,16 +519,16 @@
         <v>0</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>3</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>4</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="14"/>

</xml_diff>